<commit_message>
Testfall für ausgewählte Daten konstruiert
</commit_message>
<xml_diff>
--- a/documentation/DatenAnalyse_Datenverlust.xlsx
+++ b/documentation/DatenAnalyse_Datenverlust.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="384" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="116">
   <si>
     <t>Nummer</t>
   </si>
@@ -359,18 +359,28 @@
     <t>mini public sector</t>
   </si>
   <si>
+    <t>Kosten selected</t>
+  </si>
+  <si>
     <t>Consultants engaged, CISO appointment, incident management plan, Strong security posture</t>
+  </si>
+  <si>
+    <t>Ausgewählte Daten:</t>
+  </si>
+  <si>
+    <t>avgSelected</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt formatCode="GENERAL" numFmtId="164"/>
     <numFmt formatCode="0.00%" numFmtId="165"/>
     <numFmt formatCode="#,##0.00&quot; €&quot;" numFmtId="166"/>
     <numFmt formatCode="#,##0.00" numFmtId="167"/>
+    <numFmt formatCode="#,##0\ [$€-407];\-#,##0\ [$€-407]" numFmtId="168"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -591,10 +601,6 @@
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
-    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0">
-      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
-      <protection hidden="false" locked="true"/>
-    </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="true" applyProtection="false" borderId="0" fillId="0" fontId="8" numFmtId="164" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
@@ -624,6 +630,10 @@
       <protection hidden="false" locked="true"/>
     </xf>
     <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="167" xfId="0">
+      <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
+      <protection hidden="false" locked="true"/>
+    </xf>
+    <xf applyAlignment="false" applyBorder="false" applyFont="false" applyProtection="false" borderId="0" fillId="0" fontId="0" numFmtId="168" xfId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="false" textRotation="0" vertical="bottom" wrapText="false"/>
       <protection hidden="false" locked="true"/>
     </xf>
@@ -699,7 +709,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1139,11 +1149,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="95691926"/>
-        <c:axId val="92172274"/>
+        <c:axId val="58466156"/>
+        <c:axId val="51591148"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="95691926"/>
+        <c:axId val="58466156"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1174,7 +1184,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="92172274"/>
+        <c:crossAx val="51591148"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -1186,7 +1196,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="92172274"/>
+        <c:axId val="51591148"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1227,7 +1237,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95691926"/>
+        <c:crossAx val="58466156"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -1254,7 +1264,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1461,7 +1471,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:chart>
@@ -1646,11 +1656,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="50235576"/>
-        <c:axId val="55082309"/>
+        <c:axId val="99103847"/>
+        <c:axId val="94543881"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="50235576"/>
+        <c:axId val="99103847"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1658,7 +1668,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="55082309"/>
+        <c:crossAx val="94543881"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -1670,7 +1680,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="55082309"/>
+        <c:axId val="94543881"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1688,7 +1698,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="50235576"/>
+        <c:crossAx val="99103847"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -1720,15 +1730,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>320760</xdr:colOff>
+      <xdr:colOff>347760</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>139320</xdr:rowOff>
+      <xdr:rowOff>130320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>100800</xdr:colOff>
+      <xdr:colOff>127440</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>105120</xdr:rowOff>
+      <xdr:rowOff>95760</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1736,8 +1746,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11346840" y="520200"/>
-        <a:ext cx="11140560" cy="5490360"/>
+        <a:off x="11373840" y="511200"/>
+        <a:ext cx="11140200" cy="5490000"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1755,15 +1765,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>235080</xdr:colOff>
+      <xdr:colOff>262080</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>82440</xdr:rowOff>
+      <xdr:rowOff>73440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>234360</xdr:colOff>
+      <xdr:colOff>261000</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>157680</xdr:rowOff>
+      <xdr:rowOff>148320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1771,8 +1781,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16725960" y="5797080"/>
-        <a:ext cx="5765760" cy="2742480"/>
+        <a:off x="16752960" y="5788080"/>
+        <a:ext cx="5765400" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1785,15 +1795,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>444960</xdr:colOff>
+      <xdr:colOff>471960</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>25200</xdr:rowOff>
+      <xdr:rowOff>16200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>282240</xdr:colOff>
+      <xdr:colOff>308880</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>100440</xdr:rowOff>
+      <xdr:rowOff>91080</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1801,8 +1811,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9910080" y="5549400"/>
-        <a:ext cx="5846760" cy="2742480"/>
+        <a:off x="9937080" y="5540400"/>
+        <a:ext cx="5846400" cy="2742120"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3385,7 +3395,7 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="34">
-      <c r="C34" s="14" t="n">
+      <c r="C34" s="0" t="n">
         <f aca="false">I35+E34</f>
         <v>241</v>
       </c>
@@ -3395,7 +3405,7 @@
       <c r="E34" s="0" t="n">
         <v>90</v>
       </c>
-      <c r="F34" s="14" t="n">
+      <c r="F34" s="0" t="n">
         <f aca="false">I35-E34</f>
         <v>61</v>
       </c>
@@ -3418,47 +3428,47 @@
       <c r="B36" s="0" t="n">
         <v>5000</v>
       </c>
-      <c r="C36" s="14" t="n">
+      <c r="C36" s="0" t="n">
         <f aca="false">$C$35*B36</f>
         <v>1250000</v>
       </c>
       <c r="E36" s="0" t="n">
         <v>5000</v>
       </c>
-      <c r="F36" s="14" t="n">
+      <c r="F36" s="0" t="n">
         <f aca="false">$F$35*E36</f>
         <v>400000</v>
       </c>
       <c r="H36" s="0" t="n">
         <v>5000</v>
       </c>
-      <c r="I36" s="14" t="n">
+      <c r="I36" s="0" t="n">
         <f aca="false">$I$35*H36</f>
         <v>755000</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="37">
-      <c r="B37" s="14" t="n">
+      <c r="B37" s="0" t="n">
         <f aca="false">B36+2000</f>
         <v>7000</v>
       </c>
-      <c r="C37" s="14" t="n">
+      <c r="C37" s="0" t="n">
         <f aca="false">$C$35*B37</f>
         <v>1750000</v>
       </c>
-      <c r="E37" s="14" t="n">
+      <c r="E37" s="0" t="n">
         <f aca="false">E36+5000</f>
         <v>10000</v>
       </c>
-      <c r="F37" s="14" t="n">
+      <c r="F37" s="0" t="n">
         <f aca="false">$F$35*E37</f>
         <v>800000</v>
       </c>
-      <c r="H37" s="14" t="n">
+      <c r="H37" s="0" t="n">
         <f aca="false">H36+5000</f>
         <v>10000</v>
       </c>
-      <c r="I37" s="14" t="n">
+      <c r="I37" s="0" t="n">
         <f aca="false">$I$35*H37</f>
         <v>1510000</v>
       </c>
@@ -3467,21 +3477,21 @@
       <c r="B38" s="0" t="n">
         <v>88082</v>
       </c>
-      <c r="C38" s="14" t="n">
+      <c r="C38" s="0" t="n">
         <f aca="false">$C$35*B38</f>
         <v>22020500</v>
       </c>
       <c r="E38" s="0" t="n">
         <v>88082</v>
       </c>
-      <c r="F38" s="14" t="n">
+      <c r="F38" s="0" t="n">
         <f aca="false">$F$35*E38</f>
         <v>7046560</v>
       </c>
       <c r="H38" s="0" t="n">
         <v>88082</v>
       </c>
-      <c r="I38" s="14" t="n">
+      <c r="I38" s="0" t="n">
         <f aca="false">$I$35*H38</f>
         <v>13300382</v>
       </c>
@@ -3531,23 +3541,23 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="Q5" s="16" t="s">
+      <c r="Q5" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="R5" s="16"/>
+      <c r="R5" s="15"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
-      <c r="B6" s="15"/>
+      <c r="B6" s="14"/>
       <c r="Q6" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="R6" s="14" t="n">
+      <c r="R6" s="0" t="n">
         <f aca="false">D7</f>
         <v>512</v>
       </c>
@@ -3565,14 +3575,14 @@
       <c r="O7" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="P7" s="14" t="n">
+      <c r="P7" s="0" t="n">
         <f aca="false">D21+J19+J21+J23+J25</f>
         <v>203</v>
       </c>
       <c r="Q7" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="R7" s="17" t="n">
+      <c r="R7" s="16" t="n">
         <f aca="false">P7*D7</f>
         <v>103936</v>
       </c>
@@ -3587,14 +3597,14 @@
       <c r="O8" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="P8" s="14" t="n">
+      <c r="P8" s="0" t="n">
         <f aca="false">(E14*D21)+J19+J21+J23+J25</f>
         <v>108.490066225166</v>
       </c>
       <c r="Q8" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="R8" s="17" t="n">
+      <c r="R8" s="16" t="n">
         <f aca="false">P8*D7</f>
         <v>55546.9139072848</v>
       </c>
@@ -3609,36 +3619,36 @@
       <c r="O9" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="P9" s="14" t="n">
+      <c r="P9" s="0" t="n">
         <f aca="false">(E15*D21)+J19+J21+J23+J25</f>
         <v>334.781456953642</v>
       </c>
       <c r="Q9" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="R9" s="17" t="n">
+      <c r="R9" s="16" t="n">
         <f aca="false">P9*D7</f>
         <v>171408.105960265</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>97</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
-      <c r="O12" s="18"/>
-      <c r="P12" s="18"/>
-      <c r="Q12" s="18"/>
-      <c r="R12" s="18"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="18"/>
+      <c r="O12" s="17"/>
+      <c r="P12" s="17"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="17"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="17"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
       <c r="C13" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="R13" s="17"/>
+      <c r="R13" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
       <c r="C14" s="0" t="s">
@@ -3647,13 +3657,13 @@
       <c r="D14" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="E14" s="14" t="n">
+      <c r="E14" s="0" t="n">
         <f aca="false">D14/D16</f>
         <v>0.529801324503311</v>
       </c>
-      <c r="O14" s="17"/>
-      <c r="P14" s="17"/>
-      <c r="Q14" s="17"/>
+      <c r="O14" s="16"/>
+      <c r="P14" s="16"/>
+      <c r="Q14" s="16"/>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
@@ -3662,7 +3672,7 @@
       <c r="D15" s="0" t="n">
         <v>250</v>
       </c>
-      <c r="E15" s="14" t="n">
+      <c r="E15" s="0" t="n">
         <f aca="false">D15/D16</f>
         <v>1.65562913907285</v>
       </c>
@@ -3676,18 +3686,18 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="F18" s="19" t="s">
+      <c r="D18" s="18"/>
+      <c r="F18" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="19"/>
-      <c r="I18" s="19" t="s">
+      <c r="G18" s="18"/>
+      <c r="I18" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="J18" s="19"/>
+      <c r="J18" s="18"/>
       <c r="R18" s="0" t="s">
         <v>71</v>
       </c>
@@ -3705,33 +3715,33 @@
       <c r="D19" s="0" t="n">
         <v>217</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="21" t="n">
+      <c r="G19" s="20" t="n">
         <v>0.34</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="J19" s="20" t="n">
+      <c r="J19" s="19" t="n">
         <v>12</v>
       </c>
       <c r="M19" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="O19" s="20" t="s">
+      <c r="O19" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="R19" s="17" t="n">
+      <c r="R19" s="16" t="n">
         <f aca="false">$P$8*G19</f>
         <v>36.8866225165563</v>
       </c>
-      <c r="S19" s="17" t="n">
+      <c r="S19" s="16" t="n">
         <f aca="false">$P$7*G19</f>
         <v>69.02</v>
       </c>
-      <c r="T19" s="17" t="n">
+      <c r="T19" s="16" t="n">
         <f aca="false">$P$9*G19</f>
         <v>113.825695364238</v>
       </c>
@@ -3743,30 +3753,30 @@
       <c r="D20" s="0" t="n">
         <v>214</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="21" t="n">
+      <c r="G20" s="20" t="n">
         <v>0.29</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="20" t="n">
+      <c r="J20" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="O20" s="20" t="s">
+      <c r="O20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="R20" s="17" t="n">
+      <c r="R20" s="16" t="n">
         <f aca="false">$P$8*G20</f>
         <v>31.462119205298</v>
       </c>
-      <c r="S20" s="17" t="n">
+      <c r="S20" s="16" t="n">
         <f aca="false">$P$7*G20</f>
         <v>58.87</v>
       </c>
-      <c r="T20" s="17" t="n">
+      <c r="T20" s="16" t="n">
         <f aca="false">$P$9*G20</f>
         <v>97.0866225165563</v>
       </c>
@@ -3778,30 +3788,30 @@
       <c r="D21" s="0" t="n">
         <v>201</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G21" s="21" t="n">
+      <c r="G21" s="20" t="n">
         <v>0.09</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="J21" s="20" t="n">
+      <c r="J21" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="O21" s="20" t="s">
+      <c r="O21" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="R21" s="17" t="n">
+      <c r="R21" s="16" t="n">
         <f aca="false">$P$8*G21</f>
         <v>9.7641059602649</v>
       </c>
-      <c r="S21" s="17" t="n">
+      <c r="S21" s="16" t="n">
         <f aca="false">$P$7*G21</f>
         <v>18.27</v>
       </c>
-      <c r="T21" s="17" t="n">
+      <c r="T21" s="16" t="n">
         <f aca="false">$P$9*G21</f>
         <v>30.1303311258278</v>
       </c>
@@ -3813,30 +3823,30 @@
       <c r="D22" s="0" t="n">
         <v>161</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="21" t="n">
+      <c r="G22" s="20" t="n">
         <v>0.07</v>
       </c>
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="J22" s="20" t="n">
+      <c r="J22" s="19" t="n">
         <v>-4</v>
       </c>
-      <c r="O22" s="20" t="s">
+      <c r="O22" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="R22" s="17" t="n">
+      <c r="R22" s="16" t="n">
         <f aca="false">$P$8*G22</f>
         <v>7.59430463576159</v>
       </c>
-      <c r="S22" s="17" t="n">
+      <c r="S22" s="16" t="n">
         <f aca="false">$P$7*G22</f>
         <v>14.21</v>
       </c>
-      <c r="T22" s="17" t="n">
+      <c r="T22" s="16" t="n">
         <f aca="false">$P$9*G22</f>
         <v>23.434701986755</v>
       </c>
@@ -3848,30 +3858,30 @@
       <c r="D23" s="0" t="n">
         <v>141</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="21" t="n">
+      <c r="G23" s="20" t="n">
         <v>0.05</v>
       </c>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="J23" s="20" t="n">
+      <c r="J23" s="19" t="n">
         <v>-5</v>
       </c>
-      <c r="O23" s="20" t="s">
+      <c r="O23" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="R23" s="17" t="n">
+      <c r="R23" s="16" t="n">
         <f aca="false">$P$8*G23</f>
         <v>5.42450331125828</v>
       </c>
-      <c r="S23" s="17" t="n">
+      <c r="S23" s="16" t="n">
         <f aca="false">$P$7*G23</f>
         <v>10.15</v>
       </c>
-      <c r="T23" s="17" t="n">
+      <c r="T23" s="16" t="n">
         <f aca="false">$P$9*G23</f>
         <v>16.7390728476821</v>
       </c>
@@ -3883,30 +3893,30 @@
       <c r="D24" s="0" t="n">
         <v>134</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G24" s="21" t="n">
+      <c r="G24" s="20" t="n">
         <v>0.05</v>
       </c>
-      <c r="I24" s="20" t="s">
+      <c r="I24" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="J24" s="20" t="n">
+      <c r="J24" s="19" t="n">
         <v>-9</v>
       </c>
-      <c r="O24" s="20" t="s">
+      <c r="O24" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="R24" s="17" t="n">
+      <c r="R24" s="16" t="n">
         <f aca="false">$P$8*G24</f>
         <v>5.42450331125828</v>
       </c>
-      <c r="S24" s="17" t="n">
+      <c r="S24" s="16" t="n">
         <f aca="false">$P$7*G24</f>
         <v>10.15</v>
       </c>
-      <c r="T24" s="17" t="n">
+      <c r="T24" s="16" t="n">
         <f aca="false">$P$9*G24</f>
         <v>16.7390728476821</v>
       </c>
@@ -3918,30 +3928,30 @@
       <c r="D25" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G25" s="21" t="n">
+      <c r="G25" s="20" t="n">
         <v>0.04</v>
       </c>
-      <c r="I25" s="20" t="s">
+      <c r="I25" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="J25" s="20" t="n">
+      <c r="J25" s="19" t="n">
         <v>-11</v>
       </c>
-      <c r="O25" s="20" t="s">
+      <c r="O25" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="R25" s="17" t="n">
+      <c r="R25" s="16" t="n">
         <f aca="false">$P$8*G25</f>
         <v>4.33960264900662</v>
       </c>
-      <c r="S25" s="17" t="n">
+      <c r="S25" s="16" t="n">
         <f aca="false">$P$7*G25</f>
         <v>8.12</v>
       </c>
-      <c r="T25" s="17" t="n">
+      <c r="T25" s="16" t="n">
         <f aca="false">$P$9*G25</f>
         <v>13.3912582781457</v>
       </c>
@@ -3953,24 +3963,24 @@
       <c r="D26" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G26" s="21" t="n">
+      <c r="G26" s="20" t="n">
         <v>0.04</v>
       </c>
-      <c r="O26" s="20" t="s">
+      <c r="O26" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="R26" s="17" t="n">
+      <c r="R26" s="16" t="n">
         <f aca="false">$P$8*G26</f>
         <v>4.33960264900662</v>
       </c>
-      <c r="S26" s="17" t="n">
+      <c r="S26" s="16" t="n">
         <f aca="false">$P$7*G26</f>
         <v>8.12</v>
       </c>
-      <c r="T26" s="17" t="n">
+      <c r="T26" s="16" t="n">
         <f aca="false">$P$9*G26</f>
         <v>13.3912582781457</v>
       </c>
@@ -3982,24 +3992,24 @@
       <c r="D27" s="0" t="n">
         <v>119</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G27" s="21" t="n">
+      <c r="G27" s="20" t="n">
         <v>0.02</v>
       </c>
-      <c r="O27" s="20" t="s">
+      <c r="O27" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="R27" s="17" t="n">
+      <c r="R27" s="16" t="n">
         <f aca="false">$P$8*G27</f>
         <v>2.16980132450331</v>
       </c>
-      <c r="S27" s="17" t="n">
+      <c r="S27" s="16" t="n">
         <f aca="false">$P$7*G27</f>
         <v>4.06</v>
       </c>
-      <c r="T27" s="17" t="n">
+      <c r="T27" s="16" t="n">
         <f aca="false">$P$9*G27</f>
         <v>6.69562913907285</v>
       </c>
@@ -4011,24 +4021,24 @@
       <c r="D28" s="0" t="n">
         <v>114</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G28" s="21" t="n">
+      <c r="G28" s="20" t="n">
         <v>0.01</v>
       </c>
-      <c r="O28" s="20" t="s">
+      <c r="O28" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="R28" s="17" t="n">
+      <c r="R28" s="16" t="n">
         <f aca="false">$P$8*G28</f>
         <v>1.08490066225166</v>
       </c>
-      <c r="S28" s="17" t="n">
+      <c r="S28" s="16" t="n">
         <f aca="false">$P$7*G28</f>
         <v>2.03</v>
       </c>
-      <c r="T28" s="17" t="n">
+      <c r="T28" s="16" t="n">
         <f aca="false">$P$9*G28</f>
         <v>3.34781456953642</v>
       </c>
@@ -4040,24 +4050,24 @@
       <c r="D29" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="G29" s="21" t="n">
+      <c r="G29" s="20" t="n">
         <v>0</v>
       </c>
-      <c r="O29" s="20" t="s">
+      <c r="O29" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="R29" s="17" t="n">
+      <c r="R29" s="16" t="n">
         <f aca="false">$P$8*G29</f>
         <v>0</v>
       </c>
-      <c r="S29" s="17" t="n">
+      <c r="S29" s="16" t="n">
         <f aca="false">$P$7*G29</f>
         <v>0</v>
       </c>
-      <c r="T29" s="17" t="n">
+      <c r="T29" s="16" t="n">
         <f aca="false">$P$9*G29</f>
         <v>0</v>
       </c>
@@ -4112,15 +4122,15 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="14" t="s">
         <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
-      <c r="B6" s="15"/>
+      <c r="B6" s="14"/>
       <c r="R6" s="0" t="s">
         <v>105</v>
       </c>
@@ -4129,7 +4139,7 @@
       <c r="C7" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="22" t="n">
+      <c r="D7" s="21" t="n">
         <v>5000000</v>
       </c>
       <c r="M7" s="0" t="s">
@@ -4138,11 +4148,11 @@
       <c r="O7" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="P7" s="14" t="n">
+      <c r="P7" s="0" t="n">
         <f aca="false">D26+J20+J22+J24</f>
         <v>115</v>
       </c>
-      <c r="R7" s="17" t="n">
+      <c r="R7" s="16" t="n">
         <f aca="false">P7*D7</f>
         <v>575000000</v>
       </c>
@@ -4157,11 +4167,11 @@
       <c r="O8" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="P8" s="14" t="n">
+      <c r="P8" s="0" t="n">
         <f aca="false">(E14*D26)+J20+J22+J24</f>
         <v>58.5761589403974</v>
       </c>
-      <c r="R8" s="17" t="n">
+      <c r="R8" s="16" t="n">
         <f aca="false">P8*D7</f>
         <v>292880794.701987</v>
       </c>
@@ -4176,17 +4186,17 @@
       <c r="O9" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="P9" s="14" t="n">
+      <c r="P9" s="0" t="n">
         <f aca="false">(E15*D26)+J20+J22+J24</f>
         <v>193.675496688742</v>
       </c>
-      <c r="R9" s="17" t="n">
+      <c r="R9" s="16" t="n">
         <f aca="false">P9*D7</f>
         <v>968377483.443709</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>97</v>
       </c>
       <c r="R11" s="0" t="s">
@@ -4203,18 +4213,18 @@
       <c r="M12" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="O12" s="20" t="s">
+      <c r="O12" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="R12" s="17" t="n">
+      <c r="R12" s="16" t="n">
         <f aca="false">$P$8*G19</f>
         <v>19.9158940397351</v>
       </c>
-      <c r="S12" s="17" t="n">
+      <c r="S12" s="16" t="n">
         <f aca="false">$P$7*G19</f>
         <v>39.1</v>
       </c>
-      <c r="T12" s="17" t="n">
+      <c r="T12" s="16" t="n">
         <f aca="false">$P$9*G19</f>
         <v>65.8496688741722</v>
       </c>
@@ -4223,18 +4233,18 @@
       <c r="C13" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="O13" s="20" t="s">
+      <c r="O13" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="R13" s="17" t="n">
+      <c r="R13" s="16" t="n">
         <f aca="false">$P$8*G20</f>
         <v>16.9870860927152</v>
       </c>
-      <c r="S13" s="17" t="n">
+      <c r="S13" s="16" t="n">
         <f aca="false">$P$7*G20</f>
         <v>33.35</v>
       </c>
-      <c r="T13" s="17" t="n">
+      <c r="T13" s="16" t="n">
         <f aca="false">$P$9*G20</f>
         <v>56.1658940397351</v>
       </c>
@@ -4246,22 +4256,22 @@
       <c r="D14" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="E14" s="14" t="n">
+      <c r="E14" s="0" t="n">
         <f aca="false">D14/D16</f>
         <v>0.529801324503311</v>
       </c>
-      <c r="O14" s="20" t="s">
+      <c r="O14" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="R14" s="17" t="n">
+      <c r="R14" s="16" t="n">
         <f aca="false">$P$8*G21</f>
         <v>5.27185430463576</v>
       </c>
-      <c r="S14" s="17" t="n">
+      <c r="S14" s="16" t="n">
         <f aca="false">$P$7*G21</f>
         <v>10.35</v>
       </c>
-      <c r="T14" s="17" t="n">
+      <c r="T14" s="16" t="n">
         <f aca="false">$P$9*G21</f>
         <v>17.4307947019868</v>
       </c>
@@ -4273,22 +4283,22 @@
       <c r="D15" s="0" t="n">
         <v>250</v>
       </c>
-      <c r="E15" s="14" t="n">
+      <c r="E15" s="0" t="n">
         <f aca="false">D15/D16</f>
         <v>1.65562913907285</v>
       </c>
-      <c r="O15" s="20" t="s">
+      <c r="O15" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="R15" s="17" t="n">
+      <c r="R15" s="16" t="n">
         <f aca="false">$P$8*G22</f>
         <v>4.10033112582782</v>
       </c>
-      <c r="S15" s="17" t="n">
+      <c r="S15" s="16" t="n">
         <f aca="false">$P$7*G22</f>
         <v>8.05</v>
       </c>
-      <c r="T15" s="17" t="n">
+      <c r="T15" s="16" t="n">
         <f aca="false">$P$9*G22</f>
         <v>13.5572847682119</v>
       </c>
@@ -4300,64 +4310,64 @@
       <c r="D16" s="0" t="n">
         <v>151</v>
       </c>
-      <c r="O16" s="20" t="s">
+      <c r="O16" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="R16" s="17" t="n">
+      <c r="R16" s="16" t="n">
         <f aca="false">$P$8*G23</f>
         <v>2.92880794701987</v>
       </c>
-      <c r="S16" s="17" t="n">
+      <c r="S16" s="16" t="n">
         <f aca="false">$P$7*G23</f>
         <v>5.75</v>
       </c>
-      <c r="T16" s="17" t="n">
+      <c r="T16" s="16" t="n">
         <f aca="false">$P$9*G23</f>
         <v>9.68377483443709</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="O17" s="20" t="s">
+      <c r="O17" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="R17" s="17" t="n">
+      <c r="R17" s="16" t="n">
         <f aca="false">$P$8*G24</f>
         <v>2.92880794701987</v>
       </c>
-      <c r="S17" s="17" t="n">
+      <c r="S17" s="16" t="n">
         <f aca="false">$P$7*G24</f>
         <v>5.75</v>
       </c>
-      <c r="T17" s="17" t="n">
+      <c r="T17" s="16" t="n">
         <f aca="false">$P$9*G24</f>
         <v>9.68377483443709</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="F18" s="19" t="s">
+      <c r="D18" s="18"/>
+      <c r="F18" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="19"/>
-      <c r="I18" s="19" t="s">
+      <c r="G18" s="18"/>
+      <c r="I18" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="O18" s="20" t="s">
+      <c r="J18" s="18"/>
+      <c r="O18" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="R18" s="17" t="n">
+      <c r="R18" s="16" t="n">
         <f aca="false">$P$8*G25</f>
         <v>2.34304635761589</v>
       </c>
-      <c r="S18" s="17" t="n">
+      <c r="S18" s="16" t="n">
         <f aca="false">$P$7*G25</f>
         <v>4.6</v>
       </c>
-      <c r="T18" s="17" t="n">
+      <c r="T18" s="16" t="n">
         <f aca="false">$P$9*G25</f>
         <v>7.74701986754967</v>
       </c>
@@ -4369,30 +4379,30 @@
       <c r="D19" s="0" t="n">
         <v>217</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="21" t="n">
+      <c r="G19" s="20" t="n">
         <v>0.34</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="J19" s="20" t="n">
+      <c r="J19" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O19" s="20" t="s">
+      <c r="O19" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="R19" s="17" t="n">
+      <c r="R19" s="16" t="n">
         <f aca="false">$P$8*G26</f>
         <v>2.34304635761589</v>
       </c>
-      <c r="S19" s="17" t="n">
+      <c r="S19" s="16" t="n">
         <f aca="false">$P$7*G26</f>
         <v>4.6</v>
       </c>
-      <c r="T19" s="17" t="n">
+      <c r="T19" s="16" t="n">
         <f aca="false">$P$9*G26</f>
         <v>7.74701986754967</v>
       </c>
@@ -4404,30 +4414,30 @@
       <c r="D20" s="0" t="n">
         <v>214</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="21" t="n">
+      <c r="G20" s="20" t="n">
         <v>0.29</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="20" t="n">
+      <c r="J20" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="O20" s="20" t="s">
+      <c r="O20" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="R20" s="17" t="n">
+      <c r="R20" s="16" t="n">
         <f aca="false">$P$8*G27</f>
         <v>1.17152317880795</v>
       </c>
-      <c r="S20" s="17" t="n">
+      <c r="S20" s="16" t="n">
         <f aca="false">$P$7*G27</f>
         <v>2.3</v>
       </c>
-      <c r="T20" s="17" t="n">
+      <c r="T20" s="16" t="n">
         <f aca="false">$P$9*G27</f>
         <v>3.87350993377483</v>
       </c>
@@ -4439,30 +4449,30 @@
       <c r="D21" s="0" t="n">
         <v>201</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G21" s="21" t="n">
+      <c r="G21" s="20" t="n">
         <v>0.09</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="J21" s="20" t="n">
+      <c r="J21" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="O21" s="20" t="s">
+      <c r="O21" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="R21" s="17" t="n">
+      <c r="R21" s="16" t="n">
         <f aca="false">$P$8*G28</f>
         <v>0.585761589403974</v>
       </c>
-      <c r="S21" s="17" t="n">
+      <c r="S21" s="16" t="n">
         <f aca="false">$P$7*G28</f>
         <v>1.15</v>
       </c>
-      <c r="T21" s="17" t="n">
+      <c r="T21" s="16" t="n">
         <f aca="false">$P$9*G28</f>
         <v>1.93675496688742</v>
       </c>
@@ -4474,30 +4484,30 @@
       <c r="D22" s="0" t="n">
         <v>161</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="21" t="n">
+      <c r="G22" s="20" t="n">
         <v>0.07</v>
       </c>
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="J22" s="20" t="n">
+      <c r="J22" s="19" t="n">
         <v>-4</v>
       </c>
-      <c r="O22" s="20" t="s">
+      <c r="O22" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="R22" s="17" t="n">
+      <c r="R22" s="16" t="n">
         <f aca="false">$P$8*G29</f>
         <v>0</v>
       </c>
-      <c r="S22" s="17" t="n">
+      <c r="S22" s="16" t="n">
         <f aca="false">$P$7*G29</f>
         <v>0</v>
       </c>
-      <c r="T22" s="17" t="n">
+      <c r="T22" s="16" t="n">
         <f aca="false">$P$9*G29</f>
         <v>0</v>
       </c>
@@ -4509,16 +4519,16 @@
       <c r="D23" s="0" t="n">
         <v>141</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="21" t="n">
+      <c r="G23" s="20" t="n">
         <v>0.05</v>
       </c>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="J23" s="20" t="n">
+      <c r="J23" s="19" t="n">
         <v>-5</v>
       </c>
     </row>
@@ -4529,16 +4539,16 @@
       <c r="D24" s="0" t="n">
         <v>134</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G24" s="21" t="n">
+      <c r="G24" s="20" t="n">
         <v>0.05</v>
       </c>
-      <c r="I24" s="20" t="s">
+      <c r="I24" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="J24" s="20" t="n">
+      <c r="J24" s="19" t="n">
         <v>-9</v>
       </c>
     </row>
@@ -4549,16 +4559,16 @@
       <c r="D25" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G25" s="21" t="n">
+      <c r="G25" s="20" t="n">
         <v>0.04</v>
       </c>
-      <c r="I25" s="20" t="s">
+      <c r="I25" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="J25" s="20" t="n">
+      <c r="J25" s="19" t="n">
         <v>-11</v>
       </c>
     </row>
@@ -4569,10 +4579,10 @@
       <c r="D26" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G26" s="21" t="n">
+      <c r="G26" s="20" t="n">
         <v>0.04</v>
       </c>
     </row>
@@ -4583,10 +4593,10 @@
       <c r="D27" s="0" t="n">
         <v>119</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G27" s="21" t="n">
+      <c r="G27" s="20" t="n">
         <v>0.02</v>
       </c>
     </row>
@@ -4597,10 +4607,10 @@
       <c r="D28" s="0" t="n">
         <v>114</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G28" s="21" t="n">
+      <c r="G28" s="20" t="n">
         <v>0.01</v>
       </c>
     </row>
@@ -4611,10 +4621,10 @@
       <c r="D29" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="G29" s="21" t="n">
+      <c r="G29" s="20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4641,7 +4651,7 @@
   </sheetPr>
   <dimension ref="B3:T29"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="K1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="L1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
       <selection activeCell="M5" activeCellId="0" pane="topLeft" sqref="M5"/>
     </sheetView>
   </sheetViews>
@@ -4666,15 +4676,15 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="14" t="s">
         <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
-      <c r="B6" s="15"/>
+      <c r="B6" s="14"/>
       <c r="R6" s="0" t="s">
         <v>105</v>
       </c>
@@ -4683,7 +4693,7 @@
       <c r="C7" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="22" t="n">
+      <c r="D7" s="21" t="n">
         <v>2000000000</v>
       </c>
       <c r="M7" s="0" t="s">
@@ -4692,11 +4702,11 @@
       <c r="O7" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="P7" s="14" t="n">
+      <c r="P7" s="0" t="n">
         <f aca="false">D19+J19+J20+J21</f>
         <v>243</v>
       </c>
-      <c r="R7" s="17" t="n">
+      <c r="R7" s="16" t="n">
         <f aca="false">P7*D7</f>
         <v>486000000000</v>
       </c>
@@ -4711,11 +4721,11 @@
       <c r="O8" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="P8" s="14" t="n">
+      <c r="P8" s="0" t="n">
         <f aca="false">(E14*D19)+J19+J20+J21</f>
         <v>140.966887417219</v>
       </c>
-      <c r="R8" s="17" t="n">
+      <c r="R8" s="16" t="n">
         <f aca="false">P8*D7</f>
         <v>281933774834.437</v>
       </c>
@@ -4730,17 +4740,17 @@
       <c r="O9" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="P9" s="14" t="n">
+      <c r="P9" s="0" t="n">
         <f aca="false">(E15*D19)+J19+J20+J21</f>
         <v>385.271523178808</v>
       </c>
-      <c r="R9" s="17" t="n">
+      <c r="R9" s="16" t="n">
         <f aca="false">P9*D7</f>
         <v>770543046357.616</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>97</v>
       </c>
       <c r="R11" s="0" t="s">
@@ -4757,18 +4767,18 @@
       <c r="M12" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="O12" s="20" t="s">
+      <c r="O12" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="R12" s="17" t="n">
+      <c r="R12" s="16" t="n">
         <f aca="false">$P$8*G19</f>
         <v>47.9287417218543</v>
       </c>
-      <c r="S12" s="17" t="n">
+      <c r="S12" s="16" t="n">
         <f aca="false">$P$7*G19</f>
         <v>82.62</v>
       </c>
-      <c r="T12" s="17" t="n">
+      <c r="T12" s="16" t="n">
         <f aca="false">$P$9*G19</f>
         <v>130.992317880795</v>
       </c>
@@ -4777,18 +4787,18 @@
       <c r="C13" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="O13" s="20" t="s">
+      <c r="O13" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="R13" s="17" t="n">
+      <c r="R13" s="16" t="n">
         <f aca="false">$P$8*G20</f>
         <v>40.8803973509934</v>
       </c>
-      <c r="S13" s="17" t="n">
+      <c r="S13" s="16" t="n">
         <f aca="false">$P$7*G20</f>
         <v>70.47</v>
       </c>
-      <c r="T13" s="17" t="n">
+      <c r="T13" s="16" t="n">
         <f aca="false">$P$9*G20</f>
         <v>111.728741721854</v>
       </c>
@@ -4800,22 +4810,22 @@
       <c r="D14" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="E14" s="14" t="n">
+      <c r="E14" s="0" t="n">
         <f aca="false">D14/D16</f>
         <v>0.529801324503311</v>
       </c>
-      <c r="O14" s="20" t="s">
+      <c r="O14" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="R14" s="17" t="n">
+      <c r="R14" s="16" t="n">
         <f aca="false">$P$8*G21</f>
         <v>12.6870198675497</v>
       </c>
-      <c r="S14" s="17" t="n">
+      <c r="S14" s="16" t="n">
         <f aca="false">$P$7*G21</f>
         <v>21.87</v>
       </c>
-      <c r="T14" s="17" t="n">
+      <c r="T14" s="16" t="n">
         <f aca="false">$P$9*G21</f>
         <v>34.6744370860927</v>
       </c>
@@ -4827,22 +4837,22 @@
       <c r="D15" s="0" t="n">
         <v>250</v>
       </c>
-      <c r="E15" s="14" t="n">
+      <c r="E15" s="0" t="n">
         <f aca="false">D15/D16</f>
         <v>1.65562913907285</v>
       </c>
-      <c r="O15" s="20" t="s">
+      <c r="O15" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="R15" s="17" t="n">
+      <c r="R15" s="16" t="n">
         <f aca="false">$P$8*G22</f>
         <v>9.8676821192053</v>
       </c>
-      <c r="S15" s="17" t="n">
+      <c r="S15" s="16" t="n">
         <f aca="false">$P$7*G22</f>
         <v>17.01</v>
       </c>
-      <c r="T15" s="17" t="n">
+      <c r="T15" s="16" t="n">
         <f aca="false">$P$9*G22</f>
         <v>26.9690066225166</v>
       </c>
@@ -4854,64 +4864,64 @@
       <c r="D16" s="0" t="n">
         <v>151</v>
       </c>
-      <c r="O16" s="20" t="s">
+      <c r="O16" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="R16" s="17" t="n">
+      <c r="R16" s="16" t="n">
         <f aca="false">$P$8*G23</f>
         <v>7.04834437086093</v>
       </c>
-      <c r="S16" s="17" t="n">
+      <c r="S16" s="16" t="n">
         <f aca="false">$P$7*G23</f>
         <v>12.15</v>
       </c>
-      <c r="T16" s="17" t="n">
+      <c r="T16" s="16" t="n">
         <f aca="false">$P$9*G23</f>
         <v>19.2635761589404</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="O17" s="20" t="s">
+      <c r="O17" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="R17" s="17" t="n">
+      <c r="R17" s="16" t="n">
         <f aca="false">$P$8*G24</f>
         <v>7.04834437086093</v>
       </c>
-      <c r="S17" s="17" t="n">
+      <c r="S17" s="16" t="n">
         <f aca="false">$P$7*G24</f>
         <v>12.15</v>
       </c>
-      <c r="T17" s="17" t="n">
+      <c r="T17" s="16" t="n">
         <f aca="false">$P$9*G24</f>
         <v>19.2635761589404</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
-      <c r="C18" s="19" t="s">
+      <c r="C18" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="F18" s="19" t="s">
+      <c r="D18" s="18"/>
+      <c r="F18" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="19"/>
-      <c r="I18" s="19" t="s">
+      <c r="G18" s="18"/>
+      <c r="I18" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="O18" s="20" t="s">
+      <c r="J18" s="18"/>
+      <c r="O18" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="R18" s="17" t="n">
+      <c r="R18" s="16" t="n">
         <f aca="false">$P$8*G25</f>
         <v>5.63867549668874</v>
       </c>
-      <c r="S18" s="17" t="n">
+      <c r="S18" s="16" t="n">
         <f aca="false">$P$7*G25</f>
         <v>9.72</v>
       </c>
-      <c r="T18" s="17" t="n">
+      <c r="T18" s="16" t="n">
         <f aca="false">$P$9*G25</f>
         <v>15.4108609271523</v>
       </c>
@@ -4923,30 +4933,30 @@
       <c r="D19" s="0" t="n">
         <v>217</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="21" t="n">
+      <c r="G19" s="20" t="n">
         <v>0.34</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="J19" s="20" t="n">
+      <c r="J19" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O19" s="20" t="s">
+      <c r="O19" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="R19" s="17" t="n">
+      <c r="R19" s="16" t="n">
         <f aca="false">$P$8*G26</f>
         <v>5.63867549668874</v>
       </c>
-      <c r="S19" s="17" t="n">
+      <c r="S19" s="16" t="n">
         <f aca="false">$P$7*G26</f>
         <v>9.72</v>
       </c>
-      <c r="T19" s="17" t="n">
+      <c r="T19" s="16" t="n">
         <f aca="false">$P$9*G26</f>
         <v>15.4108609271523</v>
       </c>
@@ -4958,30 +4968,30 @@
       <c r="D20" s="0" t="n">
         <v>214</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="21" t="n">
+      <c r="G20" s="20" t="n">
         <v>0.29</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="20" t="n">
+      <c r="J20" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="O20" s="20" t="s">
+      <c r="O20" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="R20" s="17" t="n">
+      <c r="R20" s="16" t="n">
         <f aca="false">$P$8*G27</f>
         <v>2.81933774834437</v>
       </c>
-      <c r="S20" s="17" t="n">
+      <c r="S20" s="16" t="n">
         <f aca="false">$P$7*G27</f>
         <v>4.86</v>
       </c>
-      <c r="T20" s="17" t="n">
+      <c r="T20" s="16" t="n">
         <f aca="false">$P$9*G27</f>
         <v>7.70543046357616</v>
       </c>
@@ -4993,30 +5003,30 @@
       <c r="D21" s="0" t="n">
         <v>201</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G21" s="21" t="n">
+      <c r="G21" s="20" t="n">
         <v>0.09</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="J21" s="20" t="n">
+      <c r="J21" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="O21" s="20" t="s">
+      <c r="O21" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="R21" s="17" t="n">
+      <c r="R21" s="16" t="n">
         <f aca="false">$P$8*G28</f>
         <v>1.40966887417219</v>
       </c>
-      <c r="S21" s="17" t="n">
+      <c r="S21" s="16" t="n">
         <f aca="false">$P$7*G28</f>
         <v>2.43</v>
       </c>
-      <c r="T21" s="17" t="n">
+      <c r="T21" s="16" t="n">
         <f aca="false">$P$9*G28</f>
         <v>3.85271523178808</v>
       </c>
@@ -5028,30 +5038,30 @@
       <c r="D22" s="0" t="n">
         <v>161</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="21" t="n">
+      <c r="G22" s="20" t="n">
         <v>0.07</v>
       </c>
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="J22" s="20" t="n">
+      <c r="J22" s="19" t="n">
         <v>-4</v>
       </c>
-      <c r="O22" s="20" t="s">
+      <c r="O22" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="R22" s="17" t="n">
+      <c r="R22" s="16" t="n">
         <f aca="false">$P$8*G29</f>
         <v>0</v>
       </c>
-      <c r="S22" s="17" t="n">
+      <c r="S22" s="16" t="n">
         <f aca="false">$P$7*G29</f>
         <v>0</v>
       </c>
-      <c r="T22" s="17" t="n">
+      <c r="T22" s="16" t="n">
         <f aca="false">$P$9*G29</f>
         <v>0</v>
       </c>
@@ -5063,16 +5073,16 @@
       <c r="D23" s="0" t="n">
         <v>141</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="21" t="n">
+      <c r="G23" s="20" t="n">
         <v>0.05</v>
       </c>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="J23" s="20" t="n">
+      <c r="J23" s="19" t="n">
         <v>-5</v>
       </c>
     </row>
@@ -5083,16 +5093,16 @@
       <c r="D24" s="0" t="n">
         <v>134</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G24" s="21" t="n">
+      <c r="G24" s="20" t="n">
         <v>0.05</v>
       </c>
-      <c r="I24" s="20" t="s">
+      <c r="I24" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="J24" s="20" t="n">
+      <c r="J24" s="19" t="n">
         <v>-9</v>
       </c>
     </row>
@@ -5103,16 +5113,16 @@
       <c r="D25" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G25" s="21" t="n">
+      <c r="G25" s="20" t="n">
         <v>0.04</v>
       </c>
-      <c r="I25" s="20" t="s">
+      <c r="I25" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="J25" s="20" t="n">
+      <c r="J25" s="19" t="n">
         <v>-11</v>
       </c>
     </row>
@@ -5123,10 +5133,10 @@
       <c r="D26" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G26" s="21" t="n">
+      <c r="G26" s="20" t="n">
         <v>0.04</v>
       </c>
     </row>
@@ -5137,10 +5147,10 @@
       <c r="D27" s="0" t="n">
         <v>119</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G27" s="21" t="n">
+      <c r="G27" s="20" t="n">
         <v>0.02</v>
       </c>
     </row>
@@ -5151,10 +5161,10 @@
       <c r="D28" s="0" t="n">
         <v>114</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G28" s="21" t="n">
+      <c r="G28" s="20" t="n">
         <v>0.01</v>
       </c>
     </row>
@@ -5165,10 +5175,10 @@
       <c r="D29" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="G29" s="21" t="n">
+      <c r="G29" s="20" t="n">
         <v>0</v>
       </c>
     </row>
@@ -5193,10 +5203,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:T29"/>
+  <dimension ref="B3:W29"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="M5" activeCellId="0" pane="topLeft" sqref="M5"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="Q1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="X3" activeCellId="0" pane="topLeft" sqref="X3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5218,24 +5228,27 @@
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="5">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>87</v>
       </c>
-      <c r="M5" s="15" t="s">
+      <c r="M5" s="14" t="s">
         <v>88</v>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="6">
-      <c r="B6" s="15"/>
+      <c r="B6" s="14"/>
       <c r="R6" s="0" t="s">
         <v>105</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="7">
+      <c r="W6" s="0" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="7">
       <c r="C7" s="0" t="s">
         <v>90</v>
       </c>
-      <c r="D7" s="22" t="n">
+      <c r="D7" s="21" t="n">
         <v>50</v>
       </c>
       <c r="M7" s="0" t="s">
@@ -5244,16 +5257,20 @@
       <c r="O7" s="0" t="s">
         <v>91</v>
       </c>
-      <c r="P7" s="14" t="n">
+      <c r="P7" s="0" t="n">
         <f aca="false">D29+J22+J23+J24+J25</f>
         <v>64</v>
       </c>
-      <c r="R7" s="17" t="n">
+      <c r="R7" s="16" t="n">
         <f aca="false">P7*D7</f>
         <v>3200</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="8">
+      <c r="W7" s="22" t="n">
+        <f aca="false">P7*W10</f>
+        <v>1600</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="8">
       <c r="C8" s="0" t="s">
         <v>92</v>
       </c>
@@ -5263,36 +5280,52 @@
       <c r="O8" s="0" t="s">
         <v>93</v>
       </c>
-      <c r="P8" s="14" t="n">
+      <c r="P8" s="0" t="n">
         <f aca="false">(E14*D29)+J22+J23+J24+J25</f>
         <v>20.271523178808</v>
       </c>
-      <c r="R8" s="17" t="n">
+      <c r="R8" s="16" t="n">
         <f aca="false">P8*D7</f>
         <v>1013.5761589404</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="9">
+      <c r="W8" s="22" t="n">
+        <f aca="false">P8*W10</f>
+        <v>506.7880794702</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="9">
       <c r="C9" s="0" t="s">
         <v>94</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="O9" s="0" t="s">
         <v>96</v>
       </c>
-      <c r="P9" s="14" t="n">
+      <c r="P9" s="0" t="n">
         <f aca="false">(E15*D29)+J22+J23+J24+J25</f>
         <v>124.973509933775</v>
       </c>
-      <c r="R9" s="17" t="n">
+      <c r="R9" s="16" t="n">
         <f aca="false">P9*D7</f>
         <v>6248.67549668874</v>
       </c>
+      <c r="W9" s="22" t="n">
+        <f aca="false">P9*W10</f>
+        <v>3124.33774834437</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="10">
+      <c r="U10" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="W10" s="0" t="n">
+        <v>25</v>
+      </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="11">
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="14" t="s">
         <v>97</v>
       </c>
       <c r="R11" s="0" t="s">
@@ -5304,307 +5337,354 @@
       <c r="T11" s="0" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="12">
+      <c r="W11" s="0" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="12">
       <c r="M12" s="0" t="s">
         <v>103</v>
       </c>
-      <c r="O12" s="20" t="s">
+      <c r="O12" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="R12" s="17" t="n">
+      <c r="R12" s="16" t="n">
         <f aca="false">$P$8*G19</f>
         <v>6.89231788079471</v>
       </c>
-      <c r="S12" s="17" t="n">
+      <c r="S12" s="16" t="n">
         <f aca="false">$P$7*G19</f>
         <v>21.76</v>
       </c>
-      <c r="T12" s="17" t="n">
+      <c r="T12" s="16" t="n">
         <f aca="false">$P$9*G19</f>
         <v>42.4909933774835</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="13">
+      <c r="W12" s="16" t="n">
+        <f aca="false">$W$10*G19</f>
+        <v>8.5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
       <c r="C13" s="0" t="s">
         <v>98</v>
       </c>
-      <c r="O13" s="20" t="s">
+      <c r="O13" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="R13" s="17" t="n">
+      <c r="R13" s="16" t="n">
         <f aca="false">$P$8*G20</f>
         <v>5.87874172185431</v>
       </c>
-      <c r="S13" s="17" t="n">
+      <c r="S13" s="16" t="n">
         <f aca="false">$P$7*G20</f>
         <v>18.56</v>
       </c>
-      <c r="T13" s="17" t="n">
+      <c r="T13" s="16" t="n">
         <f aca="false">$P$9*G20</f>
         <v>36.2423178807947</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="14">
+      <c r="W13" s="16" t="n">
+        <f aca="false">$W$10*G20</f>
+        <v>7.25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
       <c r="C14" s="0" t="s">
         <v>71</v>
       </c>
       <c r="D14" s="0" t="n">
         <v>80</v>
       </c>
-      <c r="E14" s="14" t="n">
+      <c r="E14" s="0" t="n">
         <f aca="false">D14/D16</f>
         <v>0.529801324503311</v>
       </c>
-      <c r="O14" s="20" t="s">
+      <c r="O14" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="R14" s="17" t="n">
+      <c r="R14" s="16" t="n">
         <f aca="false">$P$8*G21</f>
         <v>1.82443708609272</v>
       </c>
-      <c r="S14" s="17" t="n">
+      <c r="S14" s="16" t="n">
         <f aca="false">$P$7*G21</f>
         <v>5.76</v>
       </c>
-      <c r="T14" s="17" t="n">
+      <c r="T14" s="16" t="n">
         <f aca="false">$P$9*G21</f>
         <v>11.2476158940397</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="15">
+      <c r="W14" s="16" t="n">
+        <f aca="false">$W$10*G21</f>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
       <c r="C15" s="0" t="s">
         <v>72</v>
       </c>
       <c r="D15" s="0" t="n">
         <v>250</v>
       </c>
-      <c r="E15" s="14" t="n">
+      <c r="E15" s="0" t="n">
         <f aca="false">D15/D16</f>
         <v>1.65562913907285</v>
       </c>
-      <c r="O15" s="20" t="s">
+      <c r="O15" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="R15" s="17" t="n">
+      <c r="R15" s="16" t="n">
         <f aca="false">$P$8*G22</f>
         <v>1.41900662251656</v>
       </c>
-      <c r="S15" s="17" t="n">
+      <c r="S15" s="16" t="n">
         <f aca="false">$P$7*G22</f>
         <v>4.48</v>
       </c>
-      <c r="T15" s="17" t="n">
+      <c r="T15" s="16" t="n">
         <f aca="false">$P$9*G22</f>
         <v>8.74814569536424</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="16">
+      <c r="W15" s="16" t="n">
+        <f aca="false">$W$10*G22</f>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
       <c r="C16" s="0" t="s">
         <v>99</v>
       </c>
       <c r="D16" s="0" t="n">
         <v>151</v>
       </c>
-      <c r="O16" s="20" t="s">
+      <c r="O16" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="R16" s="17" t="n">
+      <c r="R16" s="16" t="n">
         <f aca="false">$P$8*G23</f>
         <v>1.0135761589404</v>
       </c>
-      <c r="S16" s="17" t="n">
+      <c r="S16" s="16" t="n">
         <f aca="false">$P$7*G23</f>
         <v>3.2</v>
       </c>
-      <c r="T16" s="17" t="n">
+      <c r="T16" s="16" t="n">
         <f aca="false">$P$9*G23</f>
         <v>6.24867549668874</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="17">
-      <c r="O17" s="20" t="s">
+      <c r="W16" s="16" t="n">
+        <f aca="false">$W$10*G23</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
+      <c r="O17" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="R17" s="17" t="n">
+      <c r="R17" s="16" t="n">
         <f aca="false">$P$8*G24</f>
         <v>1.0135761589404</v>
       </c>
-      <c r="S17" s="17" t="n">
+      <c r="S17" s="16" t="n">
         <f aca="false">$P$7*G24</f>
         <v>3.2</v>
       </c>
-      <c r="T17" s="17" t="n">
+      <c r="T17" s="16" t="n">
         <f aca="false">$P$9*G24</f>
         <v>6.24867549668874</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="18">
-      <c r="C18" s="19" t="s">
+      <c r="W17" s="16" t="n">
+        <f aca="false">$W$10*G24</f>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
+      <c r="C18" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="D18" s="19"/>
-      <c r="F18" s="19" t="s">
+      <c r="D18" s="18"/>
+      <c r="F18" s="18" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="19"/>
-      <c r="I18" s="19" t="s">
+      <c r="G18" s="18"/>
+      <c r="I18" s="18" t="s">
         <v>102</v>
       </c>
-      <c r="J18" s="19"/>
-      <c r="O18" s="20" t="s">
+      <c r="J18" s="18"/>
+      <c r="O18" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="R18" s="17" t="n">
+      <c r="R18" s="16" t="n">
         <f aca="false">$P$8*G25</f>
         <v>0.810860927152318</v>
       </c>
-      <c r="S18" s="17" t="n">
+      <c r="S18" s="16" t="n">
         <f aca="false">$P$7*G25</f>
         <v>2.56</v>
       </c>
-      <c r="T18" s="17" t="n">
+      <c r="T18" s="16" t="n">
         <f aca="false">$P$9*G25</f>
         <v>4.99894039735099</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="19">
+      <c r="W18" s="16" t="n">
+        <f aca="false">$W$10*G25</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
       <c r="C19" s="0" t="s">
         <v>41</v>
       </c>
       <c r="D19" s="0" t="n">
         <v>217</v>
       </c>
-      <c r="F19" s="20" t="s">
+      <c r="F19" s="19" t="s">
         <v>43</v>
       </c>
-      <c r="G19" s="21" t="n">
+      <c r="G19" s="20" t="n">
         <v>0.34</v>
       </c>
-      <c r="I19" s="20" t="s">
+      <c r="I19" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="J19" s="20" t="n">
+      <c r="J19" s="19" t="n">
         <v>12</v>
       </c>
-      <c r="O19" s="20" t="s">
+      <c r="O19" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="R19" s="17" t="n">
+      <c r="R19" s="16" t="n">
         <f aca="false">$P$8*G26</f>
         <v>0.810860927152318</v>
       </c>
-      <c r="S19" s="17" t="n">
+      <c r="S19" s="16" t="n">
         <f aca="false">$P$7*G26</f>
         <v>2.56</v>
       </c>
-      <c r="T19" s="17" t="n">
+      <c r="T19" s="16" t="n">
         <f aca="false">$P$9*G26</f>
         <v>4.99894039735099</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="20">
+      <c r="W19" s="16" t="n">
+        <f aca="false">$W$10*G26</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
       <c r="C20" s="0" t="s">
         <v>44</v>
       </c>
       <c r="D20" s="0" t="n">
         <v>214</v>
       </c>
-      <c r="F20" s="20" t="s">
+      <c r="F20" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="21" t="n">
+      <c r="G20" s="20" t="n">
         <v>0.29</v>
       </c>
-      <c r="I20" s="20" t="s">
+      <c r="I20" s="19" t="s">
         <v>45</v>
       </c>
-      <c r="J20" s="20" t="n">
+      <c r="J20" s="19" t="n">
         <v>8</v>
       </c>
-      <c r="O20" s="20" t="s">
+      <c r="O20" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="R20" s="17" t="n">
+      <c r="R20" s="16" t="n">
         <f aca="false">$P$8*G27</f>
         <v>0.405430463576159</v>
       </c>
-      <c r="S20" s="17" t="n">
+      <c r="S20" s="16" t="n">
         <f aca="false">$P$7*G27</f>
         <v>1.28</v>
       </c>
-      <c r="T20" s="17" t="n">
+      <c r="T20" s="16" t="n">
         <f aca="false">$P$9*G27</f>
         <v>2.4994701986755</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="21">
+      <c r="W20" s="16" t="n">
+        <f aca="false">$W$10*G27</f>
+        <v>0.5</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
       <c r="C21" s="0" t="s">
         <v>47</v>
       </c>
       <c r="D21" s="0" t="n">
         <v>201</v>
       </c>
-      <c r="F21" s="20" t="s">
+      <c r="F21" s="19" t="s">
         <v>49</v>
       </c>
-      <c r="G21" s="21" t="n">
+      <c r="G21" s="20" t="n">
         <v>0.09</v>
       </c>
-      <c r="I21" s="20" t="s">
+      <c r="I21" s="19" t="s">
         <v>48</v>
       </c>
-      <c r="J21" s="20" t="n">
+      <c r="J21" s="19" t="n">
         <v>6</v>
       </c>
-      <c r="O21" s="20" t="s">
+      <c r="O21" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="R21" s="17" t="n">
+      <c r="R21" s="16" t="n">
         <f aca="false">$P$8*G28</f>
         <v>0.202715231788079</v>
       </c>
-      <c r="S21" s="17" t="n">
+      <c r="S21" s="16" t="n">
         <f aca="false">$P$7*G28</f>
         <v>0.64</v>
       </c>
-      <c r="T21" s="17" t="n">
+      <c r="T21" s="16" t="n">
         <f aca="false">$P$9*G28</f>
         <v>1.24973509933775</v>
       </c>
-    </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="22">
+      <c r="W21" s="16" t="n">
+        <f aca="false">$W$10*G28</f>
+        <v>0.25</v>
+      </c>
+    </row>
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
       <c r="C22" s="0" t="s">
         <v>50</v>
       </c>
       <c r="D22" s="0" t="n">
         <v>161</v>
       </c>
-      <c r="F22" s="20" t="s">
+      <c r="F22" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="G22" s="21" t="n">
+      <c r="G22" s="20" t="n">
         <v>0.07</v>
       </c>
-      <c r="I22" s="20" t="s">
+      <c r="I22" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="J22" s="20" t="n">
+      <c r="J22" s="19" t="n">
         <v>-4</v>
       </c>
-      <c r="O22" s="20" t="s">
+      <c r="O22" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="R22" s="17" t="n">
+      <c r="R22" s="16" t="n">
         <f aca="false">$P$8*G29</f>
         <v>0</v>
       </c>
-      <c r="S22" s="17" t="n">
+      <c r="S22" s="16" t="n">
         <f aca="false">$P$7*G29</f>
         <v>0</v>
       </c>
-      <c r="T22" s="17" t="n">
+      <c r="T22" s="16" t="n">
         <f aca="false">$P$9*G29</f>
+        <v>0</v>
+      </c>
+      <c r="W22" s="16" t="n">
+        <f aca="false">$W$10*G29</f>
         <v>0</v>
       </c>
     </row>
@@ -5615,16 +5695,16 @@
       <c r="D23" s="0" t="n">
         <v>141</v>
       </c>
-      <c r="F23" s="20" t="s">
+      <c r="F23" s="19" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="21" t="n">
+      <c r="G23" s="20" t="n">
         <v>0.05</v>
       </c>
-      <c r="I23" s="20" t="s">
+      <c r="I23" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="J23" s="20" t="n">
+      <c r="J23" s="19" t="n">
         <v>-5</v>
       </c>
     </row>
@@ -5635,16 +5715,16 @@
       <c r="D24" s="0" t="n">
         <v>134</v>
       </c>
-      <c r="F24" s="20" t="s">
+      <c r="F24" s="19" t="s">
         <v>58</v>
       </c>
-      <c r="G24" s="21" t="n">
+      <c r="G24" s="20" t="n">
         <v>0.05</v>
       </c>
-      <c r="I24" s="20" t="s">
+      <c r="I24" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="J24" s="20" t="n">
+      <c r="J24" s="19" t="n">
         <v>-9</v>
       </c>
     </row>
@@ -5655,16 +5735,16 @@
       <c r="D25" s="0" t="n">
         <v>126</v>
       </c>
-      <c r="F25" s="20" t="s">
+      <c r="F25" s="19" t="s">
         <v>61</v>
       </c>
-      <c r="G25" s="21" t="n">
+      <c r="G25" s="20" t="n">
         <v>0.04</v>
       </c>
-      <c r="I25" s="20" t="s">
+      <c r="I25" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="J25" s="20" t="n">
+      <c r="J25" s="19" t="n">
         <v>-11</v>
       </c>
     </row>
@@ -5675,10 +5755,10 @@
       <c r="D26" s="0" t="n">
         <v>120</v>
       </c>
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="G26" s="21" t="n">
+      <c r="G26" s="20" t="n">
         <v>0.04</v>
       </c>
     </row>
@@ -5689,10 +5769,10 @@
       <c r="D27" s="0" t="n">
         <v>119</v>
       </c>
-      <c r="F27" s="20" t="s">
+      <c r="F27" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G27" s="21" t="n">
+      <c r="G27" s="20" t="n">
         <v>0.02</v>
       </c>
     </row>
@@ -5703,10 +5783,10 @@
       <c r="D28" s="0" t="n">
         <v>114</v>
       </c>
-      <c r="F28" s="20" t="s">
+      <c r="F28" s="19" t="s">
         <v>67</v>
       </c>
-      <c r="G28" s="21" t="n">
+      <c r="G28" s="20" t="n">
         <v>0.01</v>
       </c>
     </row>
@@ -5717,10 +5797,10 @@
       <c r="D29" s="0" t="n">
         <v>93</v>
       </c>
-      <c r="F29" s="20" t="s">
+      <c r="F29" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="G29" s="21" t="n">
+      <c r="G29" s="20" t="n">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Datenpannen Akzeptanztest um selektierte Auswahl von Daten erweitert.
</commit_message>
<xml_diff>
--- a/documentation/DatenAnalyse_Datenverlust.xlsx
+++ b/documentation/DatenAnalyse_Datenverlust.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="6" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="484" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="6" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="221" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" state="visible" r:id="rId2"/>
@@ -380,7 +380,7 @@
     <numFmt formatCode="0.00%" numFmtId="165"/>
     <numFmt formatCode="#,##0.00&quot; €&quot;" numFmtId="166"/>
     <numFmt formatCode="#,##0.00" numFmtId="167"/>
-    <numFmt formatCode="#,##0\ [$€-407];\-#,##0\ [$€-407]" numFmtId="168"/>
+    <numFmt formatCode="#,##0.00\ [$€-407];\-#,##0.00\ [$€-407]" numFmtId="168"/>
   </numFmts>
   <fonts count="9">
     <font>
@@ -1149,11 +1149,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="58466156"/>
-        <c:axId val="51591148"/>
+        <c:axId val="92684410"/>
+        <c:axId val="62621661"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="58466156"/>
+        <c:axId val="92684410"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1184,7 +1184,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51591148"/>
+        <c:crossAx val="62621661"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -1196,7 +1196,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="51591148"/>
+        <c:axId val="62621661"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,7 +1237,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="58466156"/>
+        <c:crossAx val="92684410"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -1656,11 +1656,11 @@
             </c:numRef>
           </c:yVal>
         </c:ser>
-        <c:axId val="99103847"/>
-        <c:axId val="94543881"/>
+        <c:axId val="13762319"/>
+        <c:axId val="41013383"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="99103847"/>
+        <c:axId val="13762319"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1668,7 +1668,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="94543881"/>
+        <c:crossAx val="41013383"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -1680,7 +1680,7 @@
         </c:spPr>
       </c:valAx>
       <c:valAx>
-        <c:axId val="94543881"/>
+        <c:axId val="41013383"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1698,7 +1698,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="99103847"/>
+        <c:crossAx val="13762319"/>
         <c:crossesAt val="0"/>
         <c:spPr>
           <a:ln w="9360">
@@ -1730,15 +1730,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>347760</xdr:colOff>
+      <xdr:colOff>374760</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>130320</xdr:rowOff>
+      <xdr:rowOff>121320</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>127440</xdr:colOff>
+      <xdr:colOff>154080</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>95760</xdr:rowOff>
+      <xdr:rowOff>86400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1746,8 +1746,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="11373840" y="511200"/>
-        <a:ext cx="11140200" cy="5490000"/>
+        <a:off x="11400840" y="502200"/>
+        <a:ext cx="11139840" cy="5489640"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1765,15 +1765,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>262080</xdr:colOff>
+      <xdr:colOff>289080</xdr:colOff>
       <xdr:row>30</xdr:row>
-      <xdr:rowOff>73440</xdr:rowOff>
+      <xdr:rowOff>64440</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>19</xdr:col>
-      <xdr:colOff>261000</xdr:colOff>
+      <xdr:colOff>287640</xdr:colOff>
       <xdr:row>44</xdr:row>
-      <xdr:rowOff>148320</xdr:rowOff>
+      <xdr:rowOff>138960</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1781,8 +1781,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="16752960" y="5788080"/>
-        <a:ext cx="5765400" cy="2742120"/>
+        <a:off x="16779960" y="5779080"/>
+        <a:ext cx="5765040" cy="2741760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -1795,15 +1795,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>471960</xdr:colOff>
+      <xdr:colOff>498960</xdr:colOff>
       <xdr:row>29</xdr:row>
-      <xdr:rowOff>16200</xdr:rowOff>
+      <xdr:rowOff>7200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
-      <xdr:colOff>308880</xdr:colOff>
+      <xdr:colOff>335520</xdr:colOff>
       <xdr:row>43</xdr:row>
-      <xdr:rowOff>91080</xdr:rowOff>
+      <xdr:rowOff>81720</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -1811,8 +1811,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9937080" y="5540400"/>
-        <a:ext cx="5846400" cy="2742120"/>
+        <a:off x="9964080" y="5531400"/>
+        <a:ext cx="5846040" cy="2741760"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -4652,7 +4652,7 @@
   <dimension ref="B3:T29"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="L1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="M5" activeCellId="0" pane="topLeft" sqref="M5"/>
+      <selection activeCell="S25" activeCellId="0" pane="topLeft" sqref="S25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5205,8 +5205,8 @@
   </sheetPr>
   <dimension ref="B3:W29"/>
   <sheetViews>
-    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="Q1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="X3" activeCellId="0" pane="topLeft" sqref="X3"/>
+    <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="O1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
+      <selection activeCell="U26" activeCellId="0" pane="topLeft" sqref="U26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -5360,9 +5360,11 @@
         <f aca="false">$P$9*G19</f>
         <v>42.4909933774835</v>
       </c>
-      <c r="W12" s="16" t="n">
-        <f aca="false">$W$10*G19</f>
-        <v>8.5</v>
+      <c r="W12" s="16" t="inlineStr">
+        <f aca="false">$W$7*G19</f>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="13">
@@ -5384,9 +5386,11 @@
         <f aca="false">$P$9*G20</f>
         <v>36.2423178807947</v>
       </c>
-      <c r="W13" s="16" t="n">
-        <f aca="false">$W$10*G20</f>
-        <v>7.25</v>
+      <c r="W13" s="16" t="inlineStr">
+        <f aca="false">$W$7*G20</f>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="14">
@@ -5415,9 +5419,11 @@
         <f aca="false">$P$9*G21</f>
         <v>11.2476158940397</v>
       </c>
-      <c r="W14" s="16" t="n">
-        <f aca="false">$W$10*G21</f>
-        <v>2.25</v>
+      <c r="W14" s="16" t="inlineStr">
+        <f aca="false">$W$7*G21</f>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="15">
@@ -5446,9 +5452,11 @@
         <f aca="false">$P$9*G22</f>
         <v>8.74814569536424</v>
       </c>
-      <c r="W15" s="16" t="n">
-        <f aca="false">$W$10*G22</f>
-        <v>1.75</v>
+      <c r="W15" s="16" t="inlineStr">
+        <f aca="false">$W$7*G22</f>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="16">
@@ -5473,9 +5481,11 @@
         <f aca="false">$P$9*G23</f>
         <v>6.24867549668874</v>
       </c>
-      <c r="W16" s="16" t="n">
-        <f aca="false">$W$10*G23</f>
-        <v>1.25</v>
+      <c r="W16" s="16" t="inlineStr">
+        <f aca="false">$W$7*G23</f>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="17">
@@ -5494,9 +5504,11 @@
         <f aca="false">$P$9*G24</f>
         <v>6.24867549668874</v>
       </c>
-      <c r="W17" s="16" t="n">
-        <f aca="false">$W$10*G24</f>
-        <v>1.25</v>
+      <c r="W17" s="16" t="inlineStr">
+        <f aca="false">$W$7*G24</f>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="18">
@@ -5527,9 +5539,11 @@
         <f aca="false">$P$9*G25</f>
         <v>4.99894039735099</v>
       </c>
-      <c r="W18" s="16" t="n">
-        <f aca="false">$W$10*G25</f>
-        <v>1</v>
+      <c r="W18" s="16" t="inlineStr">
+        <f aca="false">$W$7*G25</f>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="19">
@@ -5566,9 +5580,11 @@
         <f aca="false">$P$9*G26</f>
         <v>4.99894039735099</v>
       </c>
-      <c r="W19" s="16" t="n">
-        <f aca="false">$W$10*G26</f>
-        <v>1</v>
+      <c r="W19" s="16" t="inlineStr">
+        <f aca="false">$W$7*G26</f>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="20">
@@ -5605,9 +5621,11 @@
         <f aca="false">$P$9*G27</f>
         <v>2.4994701986755</v>
       </c>
-      <c r="W20" s="16" t="n">
-        <f aca="false">$W$10*G27</f>
-        <v>0.5</v>
+      <c r="W20" s="16" t="inlineStr">
+        <f aca="false">$W$7*G27</f>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="21">
@@ -5644,9 +5662,11 @@
         <f aca="false">$P$9*G28</f>
         <v>1.24973509933775</v>
       </c>
-      <c r="W21" s="16" t="n">
-        <f aca="false">$W$10*G28</f>
-        <v>0.25</v>
+      <c r="W21" s="16" t="inlineStr">
+        <f aca="false">$W$7*G28</f>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="13.3" outlineLevel="0" r="22">
@@ -5683,9 +5703,11 @@
         <f aca="false">$P$9*G29</f>
         <v>0</v>
       </c>
-      <c r="W22" s="16" t="n">
-        <f aca="false">$W$10*G29</f>
-        <v>0</v>
+      <c r="W22" s="16" t="inlineStr">
+        <f aca="false">$W$7*G29</f>
+        <is>
+          <t/>
+        </is>
       </c>
     </row>
     <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="15" outlineLevel="0" r="23">

</xml_diff>